<commit_message>
Changes in Download profile and added to create a directory to update the profile path int the Excel
</commit_message>
<xml_diff>
--- a/Naukri_REFramework/Result/NaukriSearch.xlsx
+++ b/Naukri_REFramework/Result/NaukriSearch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sundarsi\source\RPA\UiPath\github\Naukri_REFramework\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BB953E-1928-4F3A-B068-1FA8A46FB591}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1225B35E-7044-4397-B52C-88C3082EF27B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{82030CAF-2DF0-485D-945C-EB60E8957052}"/>
   </bookViews>
@@ -545,7 +545,7 @@
         <v>7</v>
       </c>
       <c r="I2" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Modified for Email and Search input fine tuned
</commit_message>
<xml_diff>
--- a/Naukri_REFramework/Result/NaukriSearch.xlsx
+++ b/Naukri_REFramework/Result/NaukriSearch.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sundarsi\source\RPA\UiPath\github\Naukri_REFramework\Result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sundarsi\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA56D8F-D437-47D7-A909-7B0184010167}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4842FA-1BB6-4583-84B8-E1F11ADA453E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{82030CAF-2DF0-485D-945C-EB60E8957052}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>Position</t>
   </si>
@@ -139,7 +139,10 @@
     <t>15 days</t>
   </si>
   <si>
-    <t>Asp.net, C#, Angular,SQL,MVC,Java</t>
+    <t>Asp.net Developer,Full stack.Net Developer,Dotnet Developer</t>
+  </si>
+  <si>
+    <t>Asp.net, C#, Angular,SQL,MVC</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -604,10 +607,10 @@
         <v>31</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
update from VS source with latest
</commit_message>
<xml_diff>
--- a/Naukri_REFramework/Result/NaukriSearch.xlsx
+++ b/Naukri_REFramework/Result/NaukriSearch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sundarsi\me\source\RPA\UiPath\github\Naukri_REFramework\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52726611-33C2-4122-B241-2E46BCBFF67B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B03B0C-2133-48DD-8C1F-EDDA97174A0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{82030CAF-2DF0-485D-945C-EB60E8957052}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82030CAF-2DF0-485D-945C-EB60E8957052}"/>
   </bookViews>
   <sheets>
     <sheet name="NaukriSearch" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
   <si>
     <t>Position</t>
   </si>
@@ -223,22 +223,25 @@
     <t>12-15</t>
   </si>
   <si>
-    <t>Cloud Engineer</t>
-  </si>
-  <si>
-    <t>14-18</t>
-  </si>
-  <si>
-    <t>harshkumar.giroti@cai.io</t>
-  </si>
-  <si>
-    <t>Data Analytics, AWS, EC2, S3, Lambda, Auto Scaling, CI/CD, ETL, Cloudera, Hadoop, Python, Data Lakes, DevOps, Kubernetes</t>
-  </si>
-  <si>
-    <t>6-12</t>
-  </si>
-  <si>
-    <t>AWS , Python, DevOps, Data Analytics</t>
+    <t>sivaprakasam.sundaram@cai.io</t>
+  </si>
+  <si>
+    <t>Workday Support Analyst</t>
+  </si>
+  <si>
+    <t>4-10</t>
+  </si>
+  <si>
+    <t>15-20</t>
+  </si>
+  <si>
+    <t>Sitecore Developer</t>
+  </si>
+  <si>
+    <t>6-10</t>
+  </si>
+  <si>
+    <t>7-24</t>
   </si>
 </sst>
 </file>
@@ -650,25 +653,25 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="4" width="58.08984375" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="58.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -703,21 +706,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="42.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>68</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="F2" s="11">
         <v>15</v>
@@ -726,16 +729,16 @@
         <v>6</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="I2" s="11">
         <v>25</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="K2" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -749,15 +752,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B3B051-37AE-4110-A388-F82BB7F50059}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" s="5" t="s">
         <v>14</v>
       </c>
@@ -789,7 +792,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>19</v>
       </c>
@@ -821,7 +824,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>25</v>
       </c>
@@ -853,7 +856,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
@@ -885,7 +888,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="7" t="s">
         <v>31</v>
       </c>
@@ -915,7 +918,7 @@
       </c>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>1</v>
       </c>
@@ -950,7 +953,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -985,7 +988,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1020,7 +1023,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1055,7 +1058,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1090,7 +1093,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>1</v>
       </c>
@@ -1120,6 +1123,41 @@
       </c>
       <c r="J11" s="12" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>1</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="11">
+        <v>15</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="11">
+        <v>25</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1133,6 +1171,7 @@
     <hyperlink ref="K8" r:id="rId7" xr:uid="{EB9DC104-FECC-4E9C-AB8B-6E90EEE93730}"/>
     <hyperlink ref="K9" r:id="rId8" xr:uid="{16FF7FFA-2220-4535-A3ED-140261FBC8FB}"/>
     <hyperlink ref="K10" r:id="rId9" xr:uid="{8D4AB60C-BB9F-4324-A1A8-376AE6DC3DEF}"/>
+    <hyperlink ref="K12" r:id="rId10" xr:uid="{03157352-A50F-4BB0-A48B-852E18D8A033}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>